<commit_message>
add parameter calc and update parameter
</commit_message>
<xml_diff>
--- a/parameter/helper/consumption_12_23-consumption_12_to_23/log-actions-output.xlsx
+++ b/parameter/helper/consumption_12_23-consumption_12_to_23/log-actions-output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +468,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -499,16 +499,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C5" t="n">
         <v>10</v>
@@ -533,16 +533,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -553,75 +553,75 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C11" t="n">
         <v>13</v>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -641,27 +641,33 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -675,10 +681,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -689,16 +695,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -709,10 +715,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
@@ -723,10 +729,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -735,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -743,7 +749,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C18" t="n">
         <v>10</v>
@@ -757,19 +763,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -777,10 +783,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -791,16 +797,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -811,10 +817,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -825,7 +831,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="C23" t="n">
         <v>2</v>
@@ -845,10 +851,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="C24" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -859,19 +865,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -879,10 +885,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="C26" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -893,19 +899,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="C27" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
         <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -913,10 +919,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="C28" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -927,19 +933,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -947,10 +953,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="C30" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
@@ -961,16 +967,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="C31" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -981,10 +987,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -995,19 +1001,19 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C33" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
         <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1015,10 +1021,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C34" t="n">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1029,7 +1035,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>361</v>
+        <v>300</v>
       </c>
       <c r="C35" t="n">
         <v>2</v>
@@ -1038,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1049,7 +1055,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>363</v>
+        <v>302</v>
       </c>
       <c r="C36" t="n">
         <v>7</v>
@@ -1063,7 +1069,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>370</v>
+        <v>309</v>
       </c>
       <c r="C37" t="n">
         <v>10</v>
@@ -1072,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -1083,7 +1089,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="C38" t="n">
         <v>10</v>
@@ -1097,19 +1103,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>390</v>
+        <v>329</v>
       </c>
       <c r="C39" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1117,10 +1123,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>409</v>
+        <v>331</v>
       </c>
       <c r="C40" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
@@ -1131,19 +1137,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>419</v>
+        <v>340</v>
       </c>
       <c r="C41" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1151,7 +1157,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>431</v>
+        <v>365</v>
       </c>
       <c r="C42" t="n">
         <v>10</v>
@@ -1165,7 +1171,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>441</v>
+        <v>375</v>
       </c>
       <c r="C43" t="n">
         <v>2</v>
@@ -1174,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1185,7 +1191,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="C44" t="n">
         <v>7</v>
@@ -1199,7 +1205,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="C45" t="n">
         <v>2</v>
@@ -1208,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1219,7 +1225,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="C46" t="n">
         <v>7</v>
@@ -1233,10 +1239,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>459</v>
+        <v>393</v>
       </c>
       <c r="C47" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1245,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1253,7 +1259,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>468</v>
+        <v>407</v>
       </c>
       <c r="C48" t="n">
         <v>10</v>
@@ -1267,16 +1273,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>478</v>
+        <v>417</v>
       </c>
       <c r="C49" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1287,10 +1293,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>488</v>
+        <v>419</v>
       </c>
       <c r="C50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -1301,7 +1307,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>498</v>
+        <v>428</v>
       </c>
       <c r="C51" t="n">
         <v>2</v>
@@ -1310,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1321,7 +1327,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>500</v>
+        <v>430</v>
       </c>
       <c r="C52" t="n">
         <v>7</v>
@@ -1335,16 +1341,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>507</v>
+        <v>437</v>
       </c>
       <c r="C53" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>1</v>
@@ -1355,10 +1361,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>524</v>
+        <v>451</v>
       </c>
       <c r="C54" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
@@ -1369,19 +1375,19 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>554</v>
+        <v>461</v>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1389,10 +1395,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>560</v>
+        <v>475</v>
       </c>
       <c r="C56" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
@@ -1403,19 +1409,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>600</v>
+        <v>485</v>
       </c>
       <c r="C57" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1423,10 +1429,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>606</v>
+        <v>487</v>
       </c>
       <c r="C58" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
@@ -1437,19 +1443,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>616</v>
+        <v>494</v>
       </c>
       <c r="C59" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1457,10 +1463,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>622</v>
+        <v>496</v>
       </c>
       <c r="C60" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
@@ -1471,10 +1477,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>642</v>
+        <v>513</v>
       </c>
       <c r="C61" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
@@ -1483,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1491,7 +1497,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>652</v>
+        <v>537</v>
       </c>
       <c r="C62" t="n">
         <v>10</v>
@@ -1505,7 +1511,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>662</v>
+        <v>547</v>
       </c>
       <c r="C63" t="n">
         <v>2</v>
@@ -1525,7 +1531,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>664</v>
+        <v>549</v>
       </c>
       <c r="C64" t="n">
         <v>7</v>
@@ -1539,13 +1545,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>671</v>
+        <v>556</v>
       </c>
       <c r="C65" t="n">
         <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -1559,10 +1565,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>673</v>
+        <v>558</v>
       </c>
       <c r="C66" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
@@ -1573,10 +1579,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>680</v>
+        <v>567</v>
       </c>
       <c r="C67" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -1585,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1593,10 +1599,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>687</v>
+        <v>578</v>
       </c>
       <c r="C68" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
@@ -1607,19 +1613,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>707</v>
+        <v>588</v>
       </c>
       <c r="C69" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
         <v>2</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1627,10 +1633,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>712</v>
+        <v>590</v>
       </c>
       <c r="C70" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
@@ -1641,19 +1647,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>722</v>
+        <v>597</v>
       </c>
       <c r="C71" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1661,10 +1667,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>729</v>
+        <v>599</v>
       </c>
       <c r="C72" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
@@ -1675,19 +1681,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>739</v>
+        <v>648</v>
       </c>
       <c r="C73" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1695,10 +1701,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>744</v>
+        <v>650</v>
       </c>
       <c r="C74" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
@@ -1709,10 +1715,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>784</v>
+        <v>657</v>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
@@ -1721,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1729,7 +1735,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>792</v>
+        <v>680</v>
       </c>
       <c r="C76" t="n">
         <v>10</v>
@@ -1743,19 +1749,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>802</v>
+        <v>690</v>
       </c>
       <c r="C77" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1763,7 +1769,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>809</v>
+        <v>701</v>
       </c>
       <c r="C78" t="n">
         <v>10</v>
@@ -1777,16 +1783,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>819</v>
+        <v>711</v>
       </c>
       <c r="C79" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -1797,10 +1803,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>826</v>
+        <v>713</v>
       </c>
       <c r="C80" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
@@ -1811,19 +1817,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>866</v>
+        <v>720</v>
       </c>
       <c r="C81" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1831,10 +1837,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>872</v>
+        <v>722</v>
       </c>
       <c r="C82" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
@@ -1845,19 +1851,19 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>882</v>
+        <v>741</v>
       </c>
       <c r="C83" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E83" t="n">
         <v>2</v>
       </c>
       <c r="F83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1865,10 +1871,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>893</v>
+        <v>743</v>
       </c>
       <c r="C84" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
@@ -1879,16 +1885,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>903</v>
+        <v>772</v>
       </c>
       <c r="C85" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -1899,10 +1905,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>905</v>
+        <v>790</v>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
@@ -1913,7 +1919,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>912</v>
+        <v>800</v>
       </c>
       <c r="C87" t="n">
         <v>2</v>
@@ -1933,10 +1939,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>914</v>
+        <v>802</v>
       </c>
       <c r="C88" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
@@ -1947,18 +1953,324 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>931</v>
+        <v>809</v>
       </c>
       <c r="C89" t="n">
+        <v>2</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>811</v>
+      </c>
+      <c r="C90" t="n">
+        <v>7</v>
+      </c>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>818</v>
+      </c>
+      <c r="C91" t="n">
+        <v>10</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>828</v>
+      </c>
+      <c r="C92" t="n">
+        <v>60</v>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>888</v>
+      </c>
+      <c r="C93" t="n">
+        <v>2</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>890</v>
+      </c>
+      <c r="C94" t="n">
+        <v>7</v>
+      </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>897</v>
+      </c>
+      <c r="C95" t="n">
+        <v>19</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>916</v>
+      </c>
+      <c r="C96" t="n">
+        <v>10</v>
+      </c>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>926</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>928</v>
+      </c>
+      <c r="C98" t="n">
+        <v>7</v>
+      </c>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>935</v>
+      </c>
+      <c r="C99" t="n">
+        <v>2</v>
+      </c>
+      <c r="D99" t="n">
+        <v>2</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>937</v>
+      </c>
+      <c r="C100" t="n">
         <v>9</v>
       </c>
-      <c r="D89" t="n">
-        <v>0</v>
-      </c>
-      <c r="E89" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" t="n">
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>946</v>
+      </c>
+      <c r="C101" t="n">
+        <v>2</v>
+      </c>
+      <c r="D101" t="n">
+        <v>2</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>948</v>
+      </c>
+      <c r="C102" t="n">
+        <v>9</v>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>957</v>
+      </c>
+      <c r="C103" t="n">
+        <v>12</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>969</v>
+      </c>
+      <c r="C104" t="n">
+        <v>10</v>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>979</v>
+      </c>
+      <c r="C105" t="n">
+        <v>13</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>2</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>992</v>
+      </c>
+      <c r="C106" t="n">
+        <v>10</v>
+      </c>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1002</v>
+      </c>
+      <c r="C107" t="n">
+        <v>7</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update paraameter and add config nginx
</commit_message>
<xml_diff>
--- a/parameter/helper/consumption_12_23-consumption_12_to_23/log-actions-output.xlsx
+++ b/parameter/helper/consumption_12_23-consumption_12_to_23/log-actions-output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +468,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -499,16 +499,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C5" t="n">
         <v>10</v>
@@ -533,16 +533,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -553,75 +553,75 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C10" t="n">
-        <v>12</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C11" t="n">
         <v>13</v>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -641,33 +641,27 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C13" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -681,10 +675,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -695,16 +689,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -715,10 +709,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
@@ -729,10 +723,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="C17" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -741,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -749,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C18" t="n">
         <v>10</v>
@@ -763,19 +757,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -783,10 +777,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -797,16 +791,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -817,10 +811,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -831,7 +825,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="C23" t="n">
         <v>2</v>
@@ -851,10 +845,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -865,19 +859,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -885,10 +879,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="C26" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -899,19 +893,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -919,10 +913,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C28" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -933,19 +927,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -953,10 +947,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C30" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
@@ -967,16 +961,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -987,10 +981,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -1001,19 +995,19 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C33" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
         <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1021,10 +1015,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1035,7 +1029,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>300</v>
+        <v>361</v>
       </c>
       <c r="C35" t="n">
         <v>2</v>
@@ -1044,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1055,7 +1049,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>302</v>
+        <v>363</v>
       </c>
       <c r="C36" t="n">
         <v>7</v>
@@ -1069,7 +1063,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>309</v>
+        <v>370</v>
       </c>
       <c r="C37" t="n">
         <v>10</v>
@@ -1078,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -1089,7 +1083,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>319</v>
+        <v>380</v>
       </c>
       <c r="C38" t="n">
         <v>10</v>
@@ -1103,19 +1097,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>329</v>
+        <v>390</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1123,10 +1117,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>331</v>
+        <v>409</v>
       </c>
       <c r="C40" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
@@ -1137,19 +1131,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>340</v>
+        <v>419</v>
       </c>
       <c r="C41" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1157,7 +1151,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>365</v>
+        <v>431</v>
       </c>
       <c r="C42" t="n">
         <v>10</v>
@@ -1171,7 +1165,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>375</v>
+        <v>441</v>
       </c>
       <c r="C43" t="n">
         <v>2</v>
@@ -1180,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1191,7 +1185,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>377</v>
+        <v>443</v>
       </c>
       <c r="C44" t="n">
         <v>7</v>
@@ -1205,7 +1199,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>384</v>
+        <v>450</v>
       </c>
       <c r="C45" t="n">
         <v>2</v>
@@ -1214,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1225,7 +1219,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="C46" t="n">
         <v>7</v>
@@ -1239,10 +1233,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>393</v>
+        <v>459</v>
       </c>
       <c r="C47" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1251,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1259,7 +1253,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>407</v>
+        <v>468</v>
       </c>
       <c r="C48" t="n">
         <v>10</v>
@@ -1273,16 +1267,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>417</v>
+        <v>478</v>
       </c>
       <c r="C49" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1293,10 +1287,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>419</v>
+        <v>488</v>
       </c>
       <c r="C50" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -1307,7 +1301,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>428</v>
+        <v>498</v>
       </c>
       <c r="C51" t="n">
         <v>2</v>
@@ -1316,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1327,7 +1321,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="C52" t="n">
         <v>7</v>
@@ -1341,16 +1335,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>437</v>
+        <v>507</v>
       </c>
       <c r="C53" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>1</v>
@@ -1361,10 +1355,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>451</v>
+        <v>524</v>
       </c>
       <c r="C54" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
@@ -1375,19 +1369,19 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>461</v>
+        <v>554</v>
       </c>
       <c r="C55" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1395,10 +1389,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>475</v>
+        <v>560</v>
       </c>
       <c r="C56" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
@@ -1409,19 +1403,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>485</v>
+        <v>600</v>
       </c>
       <c r="C57" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1429,10 +1423,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>487</v>
+        <v>606</v>
       </c>
       <c r="C58" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
@@ -1443,19 +1437,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>494</v>
+        <v>616</v>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1463,10 +1457,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>496</v>
+        <v>622</v>
       </c>
       <c r="C60" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
@@ -1477,10 +1471,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>513</v>
+        <v>642</v>
       </c>
       <c r="C61" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
@@ -1489,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1497,7 +1491,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>537</v>
+        <v>652</v>
       </c>
       <c r="C62" t="n">
         <v>10</v>
@@ -1511,7 +1505,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>547</v>
+        <v>662</v>
       </c>
       <c r="C63" t="n">
         <v>2</v>
@@ -1531,7 +1525,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>549</v>
+        <v>664</v>
       </c>
       <c r="C64" t="n">
         <v>7</v>
@@ -1545,13 +1539,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>556</v>
+        <v>671</v>
       </c>
       <c r="C65" t="n">
         <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -1565,10 +1559,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>558</v>
+        <v>673</v>
       </c>
       <c r="C66" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
@@ -1579,10 +1573,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>567</v>
+        <v>680</v>
       </c>
       <c r="C67" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -1591,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1599,10 +1593,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>578</v>
+        <v>687</v>
       </c>
       <c r="C68" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
@@ -1613,19 +1607,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>588</v>
+        <v>707</v>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
         <v>2</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1633,10 +1627,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>590</v>
+        <v>712</v>
       </c>
       <c r="C70" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
@@ -1647,19 +1641,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>597</v>
+        <v>722</v>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1667,10 +1661,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>599</v>
+        <v>729</v>
       </c>
       <c r="C72" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
@@ -1681,19 +1675,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>648</v>
+        <v>739</v>
       </c>
       <c r="C73" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1701,10 +1695,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>650</v>
+        <v>744</v>
       </c>
       <c r="C74" t="n">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
@@ -1715,10 +1709,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>657</v>
+        <v>784</v>
       </c>
       <c r="C75" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
@@ -1727,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -1735,7 +1729,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>680</v>
+        <v>792</v>
       </c>
       <c r="C76" t="n">
         <v>10</v>
@@ -1749,19 +1743,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>690</v>
+        <v>802</v>
       </c>
       <c r="C77" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1769,7 +1763,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>701</v>
+        <v>809</v>
       </c>
       <c r="C78" t="n">
         <v>10</v>
@@ -1783,16 +1777,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>711</v>
+        <v>819</v>
       </c>
       <c r="C79" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -1803,10 +1797,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>713</v>
+        <v>826</v>
       </c>
       <c r="C80" t="n">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
@@ -1817,19 +1811,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>720</v>
+        <v>866</v>
       </c>
       <c r="C81" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D81" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1837,10 +1831,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>722</v>
+        <v>872</v>
       </c>
       <c r="C82" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
@@ -1851,19 +1845,19 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>741</v>
+        <v>882</v>
       </c>
       <c r="C83" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E83" t="n">
         <v>2</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -1871,10 +1865,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>743</v>
+        <v>893</v>
       </c>
       <c r="C84" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
@@ -1885,16 +1879,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>772</v>
+        <v>903</v>
       </c>
       <c r="C85" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -1905,10 +1899,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>790</v>
+        <v>905</v>
       </c>
       <c r="C86" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
@@ -1919,7 +1913,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>800</v>
+        <v>912</v>
       </c>
       <c r="C87" t="n">
         <v>2</v>
@@ -1939,10 +1933,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>802</v>
+        <v>914</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
@@ -1953,324 +1947,18 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>809</v>
+        <v>931</v>
       </c>
       <c r="C89" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="n">
         <v>2</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="n">
-        <v>811</v>
-      </c>
-      <c r="C90" t="n">
-        <v>7</v>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="n">
-        <v>818</v>
-      </c>
-      <c r="C91" t="n">
-        <v>10</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0</v>
-      </c>
-      <c r="F91" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="n">
-        <v>828</v>
-      </c>
-      <c r="C92" t="n">
-        <v>60</v>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>888</v>
-      </c>
-      <c r="C93" t="n">
-        <v>2</v>
-      </c>
-      <c r="D93" t="n">
-        <v>1</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>890</v>
-      </c>
-      <c r="C94" t="n">
-        <v>7</v>
-      </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>897</v>
-      </c>
-      <c r="C95" t="n">
-        <v>19</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0</v>
-      </c>
-      <c r="E95" t="n">
-        <v>2</v>
-      </c>
-      <c r="F95" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="n">
-        <v>916</v>
-      </c>
-      <c r="C96" t="n">
-        <v>10</v>
-      </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="n">
-        <v>926</v>
-      </c>
-      <c r="C97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1</v>
-      </c>
-      <c r="E97" t="n">
-        <v>2</v>
-      </c>
-      <c r="F97" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="n">
-        <v>928</v>
-      </c>
-      <c r="C98" t="n">
-        <v>7</v>
-      </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="n">
-        <v>935</v>
-      </c>
-      <c r="C99" t="n">
-        <v>2</v>
-      </c>
-      <c r="D99" t="n">
-        <v>2</v>
-      </c>
-      <c r="E99" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="n">
-        <v>937</v>
-      </c>
-      <c r="C100" t="n">
-        <v>9</v>
-      </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>946</v>
-      </c>
-      <c r="C101" t="n">
-        <v>2</v>
-      </c>
-      <c r="D101" t="n">
-        <v>2</v>
-      </c>
-      <c r="E101" t="n">
-        <v>2</v>
-      </c>
-      <c r="F101" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="n">
-        <v>948</v>
-      </c>
-      <c r="C102" t="n">
-        <v>9</v>
-      </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
-      <c r="F102" t="inlineStr"/>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="n">
-        <v>957</v>
-      </c>
-      <c r="C103" t="n">
-        <v>12</v>
-      </c>
-      <c r="D103" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0</v>
-      </c>
-      <c r="F103" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="n">
-        <v>969</v>
-      </c>
-      <c r="C104" t="n">
-        <v>10</v>
-      </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="n">
-        <v>979</v>
-      </c>
-      <c r="C105" t="n">
-        <v>13</v>
-      </c>
-      <c r="D105" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" t="n">
-        <v>2</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="n">
-        <v>992</v>
-      </c>
-      <c r="C106" t="n">
-        <v>10</v>
-      </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="n">
-        <v>1002</v>
-      </c>
-      <c r="C107" t="n">
-        <v>7</v>
-      </c>
-      <c r="D107" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0</v>
-      </c>
-      <c r="F107" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>